<commit_message>
adding stuff for actual data and display
</commit_message>
<xml_diff>
--- a/assets/doggo.xlsx
+++ b/assets/doggo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Royce\Desktop\Web Dev\Doggo Dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Royce\Desktop\Web Dev\doggodictionary\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,24 +24,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>word</t>
   </si>
   <si>
-    <t>def</t>
-  </si>
-  <si>
     <t>doggo</t>
   </si>
   <si>
-    <t>big pupper</t>
-  </si>
-  <si>
     <t>pupper</t>
   </si>
   <si>
     <t>smol doggo</t>
+  </si>
+  <si>
+    <t>is a full-size pupper</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>pos</t>
+  </si>
+  <si>
+    <t>noun</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>assets/images/placeholder.png</t>
   </si>
 </sst>
 </file>
@@ -359,40 +371,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="D3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>